<commit_message>
New Shunt Cal sheets for the small scale LBCBs
</commit_message>
<xml_diff>
--- a/Config/Calibrations/OneFifthBox1DisplacementCals.xlsx
+++ b/Config/Calibrations/OneFifthBox1DisplacementCals.xlsx
@@ -1,17 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22416"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="135" windowWidth="18195" windowHeight="9525"/>
+    <workbookView xWindow="240" yWindow="140" windowWidth="20140" windowHeight="16800"/>
   </bookViews>
   <sheets>
     <sheet name="Displacement Cals" sheetId="1" r:id="rId1"/>
     <sheet name="SW Cmd Cals" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -180,9 +185,6 @@
   </cellStyleXfs>
   <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -190,6 +192,9 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="3"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -595,33 +600,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:G64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="G62" sqref="G62"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F65" sqref="F65"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="15.7109375" customWidth="1"/>
-    <col min="3" max="3" width="18.28515625" customWidth="1"/>
-    <col min="4" max="4" width="21.42578125" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" customWidth="1"/>
+    <col min="3" max="3" width="18.33203125" customWidth="1"/>
+    <col min="4" max="4" width="21.5" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="8" t="s">
+    <row r="2" spans="2:7" ht="20" thickBot="1">
+      <c r="B2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8" t="s">
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-    </row>
-    <row r="3" spans="2:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+    </row>
+    <row r="3" spans="2:7" ht="15" thickTop="1">
       <c r="B3" t="s">
         <v>6</v>
       </c>
@@ -641,7 +646,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:7">
       <c r="B4">
         <v>0</v>
       </c>
@@ -661,7 +666,7 @@
         <v>3.5960000000000001</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:7">
       <c r="B5">
         <v>1</v>
       </c>
@@ -681,7 +686,7 @@
         <v>3.3279999999999998</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:7">
       <c r="B6">
         <v>2</v>
       </c>
@@ -701,7 +706,7 @@
         <v>3.0590000000000002</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:7">
       <c r="B7">
         <v>3</v>
       </c>
@@ -721,7 +726,7 @@
         <v>2.7919999999999998</v>
       </c>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:7">
       <c r="B8">
         <v>2</v>
       </c>
@@ -741,7 +746,7 @@
         <v>3.0619999999999998</v>
       </c>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:7">
       <c r="B9">
         <v>1</v>
       </c>
@@ -761,7 +766,7 @@
         <v>3.3279999999999998</v>
       </c>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:7">
       <c r="B10">
         <v>0</v>
       </c>
@@ -774,14 +779,14 @@
       <c r="E10">
         <v>0</v>
       </c>
-      <c r="F10" s="6">
+      <c r="F10" s="5">
         <v>-4.0047299999999997E-3</v>
       </c>
       <c r="G10">
         <v>3.5990000000000002</v>
       </c>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:7">
       <c r="B11">
         <v>-1</v>
       </c>
@@ -801,7 +806,7 @@
         <v>3.8839999999999999</v>
       </c>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:7">
       <c r="B12">
         <v>-2</v>
       </c>
@@ -821,7 +826,7 @@
         <v>4.1379999999999999</v>
       </c>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:7">
       <c r="B13">
         <v>-3</v>
       </c>
@@ -841,7 +846,7 @@
         <v>4.4080000000000004</v>
       </c>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:7">
       <c r="B14">
         <v>-2</v>
       </c>
@@ -861,7 +866,7 @@
         <v>4.1340000000000003</v>
       </c>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:7">
       <c r="B15">
         <v>-1</v>
       </c>
@@ -881,7 +886,7 @@
         <v>3.867</v>
       </c>
     </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:7">
       <c r="B16">
         <v>0</v>
       </c>
@@ -901,39 +906,39 @@
         <v>3.593</v>
       </c>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B17" s="5" t="s">
+    <row r="17" spans="2:7">
+      <c r="B17" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C17" s="7">
+      <c r="C17" s="6">
         <f>SLOPE(D4:D16,B4:B16)</f>
         <v>-0.26832894736842106</v>
       </c>
-      <c r="D17" s="7">
+      <c r="D17" s="6">
         <f>SLOPE(D4:D16,C4:C16)</f>
         <v>0.26813377528826898</v>
       </c>
-      <c r="E17" s="5" t="s">
+      <c r="E17" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="F17" s="7">
+      <c r="F17" s="6">
         <f>SLOPE(G4:G16,E4:E16)</f>
         <v>-0.26960526315789474</v>
       </c>
-      <c r="G17" s="7">
+      <c r="G17" s="6">
         <f>SLOPE(G4:G16,F4:F16)</f>
         <v>0.27107746097929092</v>
       </c>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B18" s="5"/>
+    <row r="18" spans="2:7">
+      <c r="B18" s="4"/>
       <c r="C18" t="s">
         <v>2</v>
       </c>
       <c r="D18" t="s">
         <v>3</v>
       </c>
-      <c r="E18" s="5"/>
+      <c r="E18" s="4"/>
       <c r="F18" t="s">
         <v>2</v>
       </c>
@@ -941,8 +946,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B19" s="5" t="s">
+    <row r="19" spans="2:7">
+      <c r="B19" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C19">
@@ -953,7 +958,7 @@
         <f>RSQ(D4:D16,C4:C16)</f>
         <v>0.99998802191634484</v>
       </c>
-      <c r="E19" s="5" t="s">
+      <c r="E19" s="4" t="s">
         <v>4</v>
       </c>
       <c r="F19">
@@ -965,87 +970,87 @@
         <v>0.9998984959286098</v>
       </c>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B20" s="5" t="s">
+    <row r="20" spans="2:7">
+      <c r="B20" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C20">
-        <v>-0.26889473684210524</v>
+        <v>-0.26734361718872979</v>
       </c>
       <c r="D20">
-        <v>0.26773623149939174</v>
-      </c>
-      <c r="E20" s="5" t="s">
+        <v>0.26732885080511981</v>
+      </c>
+      <c r="E20" s="4" t="s">
         <v>5</v>
       </c>
       <c r="F20">
-        <v>-0.26820424107142854</v>
+        <v>-0.27068181818181819</v>
       </c>
       <c r="G20">
-        <v>0.26755083133801272</v>
-      </c>
-    </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B21" s="5" t="s">
+        <v>0.27179659542604756</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7">
+      <c r="B21" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C21">
         <f>C17-C20</f>
-        <v>5.6578947368418619E-4</v>
+        <v>-9.8533017969126835E-4</v>
       </c>
       <c r="D21">
         <f>D17-D20</f>
-        <v>3.9754378887724151E-4</v>
-      </c>
-      <c r="E21" s="5" t="s">
+        <v>8.0492448314917198E-4</v>
+      </c>
+      <c r="E21" s="4" t="s">
         <v>9</v>
       </c>
       <c r="F21">
         <f>F17-F20</f>
-        <v>-1.4010220864661971E-3</v>
+        <v>1.0765550239234534E-3</v>
       </c>
       <c r="G21">
         <f>G17-G20</f>
-        <v>3.5266296412782006E-3</v>
-      </c>
-    </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B22" s="5" t="s">
+        <v>-7.1913444675664184E-4</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7">
+      <c r="B22" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C22" s="2">
+      <c r="C22" s="1">
         <f>(C20-C17)/((C17+C20)/2)</f>
-        <v>2.1063459795732523E-3</v>
-      </c>
-      <c r="D22" s="2">
+        <v>-3.6788525113503122E-3</v>
+      </c>
+      <c r="D22" s="1">
         <f>(D20-D17)/((D17+D20)/2)</f>
-        <v>-1.4837321881863369E-3</v>
-      </c>
-      <c r="E22" s="5" t="s">
+        <v>-3.0064637340675463E-3</v>
+      </c>
+      <c r="E22" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F22" s="2">
+      <c r="F22" s="1">
         <f>(F20-F17)/((F17+F20)/2)</f>
-        <v>-5.2101053456608233E-3</v>
-      </c>
-      <c r="G22" s="2">
+        <v>3.9851222104144834E-3</v>
+      </c>
+      <c r="G22" s="1">
         <f>(G20-G17)/((G17+G20)/2)</f>
-        <v>-1.3094854806478224E-2</v>
-      </c>
-    </row>
-    <row r="23" spans="2:7" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="8" t="s">
+        <v>2.649360153691699E-3</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" ht="20" thickBot="1">
+      <c r="B23" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C23" s="8"/>
-      <c r="D23" s="8"/>
-      <c r="E23" s="8" t="s">
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="F23" s="8"/>
-      <c r="G23" s="8"/>
-    </row>
-    <row r="24" spans="2:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="F23" s="7"/>
+      <c r="G23" s="7"/>
+    </row>
+    <row r="24" spans="2:7" ht="15" thickTop="1">
       <c r="B24" t="s">
         <v>6</v>
       </c>
@@ -1065,7 +1070,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:7">
       <c r="B25">
         <v>0</v>
       </c>
@@ -1085,7 +1090,7 @@
         <v>2.5910000000000002</v>
       </c>
     </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:7">
       <c r="B26">
         <v>1</v>
       </c>
@@ -1105,7 +1110,7 @@
         <v>2.4590000000000001</v>
       </c>
     </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:7">
       <c r="B27">
         <v>2</v>
       </c>
@@ -1125,7 +1130,7 @@
         <v>2.3260000000000001</v>
       </c>
     </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:7">
       <c r="B28">
         <v>3</v>
       </c>
@@ -1145,7 +1150,7 @@
         <v>2.1970000000000001</v>
       </c>
     </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:7">
       <c r="B29">
         <v>2</v>
       </c>
@@ -1165,7 +1170,7 @@
         <v>2.327</v>
       </c>
     </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:7">
       <c r="B30">
         <v>1</v>
       </c>
@@ -1185,7 +1190,7 @@
         <v>2.464</v>
       </c>
     </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:7">
       <c r="B31">
         <v>0</v>
       </c>
@@ -1205,7 +1210,7 @@
         <v>2.589</v>
       </c>
     </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:7">
       <c r="B32">
         <v>-1</v>
       </c>
@@ -1225,7 +1230,7 @@
         <v>2.7210000000000001</v>
       </c>
     </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:7">
       <c r="B33">
         <v>-2</v>
       </c>
@@ -1245,7 +1250,7 @@
         <v>2.85</v>
       </c>
     </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:7">
       <c r="B34">
         <v>-3</v>
       </c>
@@ -1265,7 +1270,7 @@
         <v>2.984</v>
       </c>
     </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:7">
       <c r="B35">
         <v>-2</v>
       </c>
@@ -1285,7 +1290,7 @@
         <v>2.8490000000000002</v>
       </c>
     </row>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:7">
       <c r="B36">
         <v>-1</v>
       </c>
@@ -1305,7 +1310,7 @@
         <v>2.7189999999999999</v>
       </c>
     </row>
-    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:7">
       <c r="B37">
         <v>0</v>
       </c>
@@ -1325,39 +1330,39 @@
         <v>2.585</v>
       </c>
     </row>
-    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B38" s="5" t="s">
+    <row r="38" spans="2:7">
+      <c r="B38" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C38" s="7">
+      <c r="C38" s="6">
         <f>SLOPE(D25:D37,B25:B37)</f>
         <v>-0.13186842105263161</v>
       </c>
-      <c r="D38" s="7">
+      <c r="D38" s="6">
         <f>SLOPE(D25:D37,C25:C37)</f>
         <v>0.13165577242448601</v>
       </c>
-      <c r="E38" s="5" t="s">
+      <c r="E38" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="F38" s="7">
+      <c r="F38" s="6">
         <f>SLOPE(G25:G37,E25:E37)</f>
         <v>-0.13078947368421051</v>
       </c>
-      <c r="G38" s="7">
+      <c r="G38" s="6">
         <f>SLOPE(G25:G37,F25:F37)</f>
         <v>0.13161843383396685</v>
       </c>
     </row>
-    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B39" s="5"/>
+    <row r="39" spans="2:7">
+      <c r="B39" s="4"/>
       <c r="C39" t="s">
         <v>2</v>
       </c>
       <c r="D39" t="s">
         <v>3</v>
       </c>
-      <c r="E39" s="5"/>
+      <c r="E39" s="4"/>
       <c r="F39" t="s">
         <v>2</v>
       </c>
@@ -1365,8 +1370,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B40" s="5" t="s">
+    <row r="40" spans="2:7">
+      <c r="B40" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C40">
@@ -1377,7 +1382,7 @@
         <f>RSQ(D25:D37,C25:C37)</f>
         <v>0.99989907425655244</v>
       </c>
-      <c r="E40" s="5" t="s">
+      <c r="E40" s="4" t="s">
         <v>4</v>
       </c>
       <c r="F40">
@@ -1389,87 +1394,87 @@
         <v>0.99990209168014954</v>
       </c>
     </row>
-    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B41" s="5" t="s">
+    <row r="41" spans="2:7">
+      <c r="B41" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C41">
-        <v>-0.13434415584415585</v>
+        <v>-0.12935563380281689</v>
       </c>
       <c r="D41">
-        <v>0.13501478873891026</v>
-      </c>
-      <c r="E41" s="5" t="s">
+        <v>0.12925345471864672</v>
+      </c>
+      <c r="E41" s="4" t="s">
         <v>5</v>
       </c>
       <c r="F41">
-        <v>-0.13429232283464571</v>
+        <v>-0.1312823660714286</v>
       </c>
       <c r="G41">
-        <v>0.13519771607008962</v>
-      </c>
-    </row>
-    <row r="42" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B42" s="5" t="s">
+        <v>0.13208895570119597</v>
+      </c>
+    </row>
+    <row r="42" spans="2:7">
+      <c r="B42" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C42">
         <f>C38-C41</f>
-        <v>2.4757347915242423E-3</v>
+        <v>-2.512787249814713E-3</v>
       </c>
       <c r="D42">
         <f>D38-D41</f>
-        <v>-3.3590163144242569E-3</v>
-      </c>
-      <c r="E42" s="5" t="s">
+        <v>2.4023177058392908E-3</v>
+      </c>
+      <c r="E42" s="4" t="s">
         <v>9</v>
       </c>
       <c r="F42">
         <f>F38-F41</f>
-        <v>3.5028491504351944E-3</v>
+        <v>4.928923872180857E-4</v>
       </c>
       <c r="G42">
         <f>G38-G41</f>
-        <v>-3.5792822361227772E-3</v>
-      </c>
-    </row>
-    <row r="43" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B43" s="5" t="s">
+        <v>-4.7052186722912337E-4</v>
+      </c>
+    </row>
+    <row r="43" spans="2:7">
+      <c r="B43" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C43" s="2">
+      <c r="C43" s="1">
         <f>(C41-C38)/((C38+C41)/2)</f>
-        <v>1.8599683158351324E-2</v>
-      </c>
-      <c r="D43" s="2">
+        <v>-1.9238559413720102E-2</v>
+      </c>
+      <c r="D43" s="1">
         <f>(D41-D38)/((D38+D41)/2)</f>
-        <v>2.5192254441359929E-2</v>
-      </c>
-      <c r="E43" s="5" t="s">
+        <v>-1.8414969314376903E-2</v>
+      </c>
+      <c r="E43" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F43" s="2">
+      <c r="F43" s="1">
         <f>(F41-F38)/((F38+F41)/2)</f>
-        <v>2.6428439798098502E-2</v>
-      </c>
-      <c r="G43" s="2">
+        <v>3.7615059113384193E-3</v>
+      </c>
+      <c r="G43" s="1">
         <f>(G41-G38)/((G38+G41)/2)</f>
-        <v>2.6829577125746247E-2</v>
-      </c>
-    </row>
-    <row r="44" spans="2:7" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B44" s="8" t="s">
+        <v>3.5685148456288053E-3</v>
+      </c>
+    </row>
+    <row r="44" spans="2:7" ht="20" thickBot="1">
+      <c r="B44" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C44" s="8"/>
-      <c r="D44" s="8"/>
-      <c r="E44" s="8" t="s">
+      <c r="C44" s="7"/>
+      <c r="D44" s="7"/>
+      <c r="E44" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="F44" s="8"/>
-      <c r="G44" s="8"/>
-    </row>
-    <row r="45" spans="2:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="F44" s="7"/>
+      <c r="G44" s="7"/>
+    </row>
+    <row r="45" spans="2:7" ht="15" thickTop="1">
       <c r="B45" t="s">
         <v>6</v>
       </c>
@@ -1489,7 +1494,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="46" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:7">
       <c r="B46">
         <v>0</v>
       </c>
@@ -1509,7 +1514,7 @@
         <v>2.59</v>
       </c>
     </row>
-    <row r="47" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:7">
       <c r="B47">
         <v>1</v>
       </c>
@@ -1529,7 +1534,7 @@
         <v>2.4569999999999999</v>
       </c>
     </row>
-    <row r="48" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:7">
       <c r="B48">
         <v>2</v>
       </c>
@@ -1549,7 +1554,7 @@
         <v>2.319</v>
       </c>
     </row>
-    <row r="49" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:7">
       <c r="B49">
         <v>3</v>
       </c>
@@ -1569,7 +1574,7 @@
         <v>2.1850000000000001</v>
       </c>
     </row>
-    <row r="50" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:7">
       <c r="B50">
         <v>2</v>
       </c>
@@ -1589,7 +1594,7 @@
         <v>2.3199999999999998</v>
       </c>
     </row>
-    <row r="51" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:7">
       <c r="B51">
         <v>1</v>
       </c>
@@ -1609,7 +1614,7 @@
         <v>2.4550000000000001</v>
       </c>
     </row>
-    <row r="52" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:7">
       <c r="B52">
         <v>0</v>
       </c>
@@ -1629,7 +1634,7 @@
         <v>2.59</v>
       </c>
     </row>
-    <row r="53" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:7">
       <c r="B53">
         <v>-1</v>
       </c>
@@ -1649,7 +1654,7 @@
         <v>2.7250000000000001</v>
       </c>
     </row>
-    <row r="54" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:7">
       <c r="B54">
         <v>-2</v>
       </c>
@@ -1669,7 +1674,7 @@
         <v>2.863</v>
       </c>
     </row>
-    <row r="55" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:7">
       <c r="B55">
         <v>-3</v>
       </c>
@@ -1689,7 +1694,7 @@
         <v>2.9990000000000001</v>
       </c>
     </row>
-    <row r="56" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:7">
       <c r="B56">
         <v>-2</v>
       </c>
@@ -1709,7 +1714,7 @@
         <v>2.8610000000000002</v>
       </c>
     </row>
-    <row r="57" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:7">
       <c r="B57">
         <v>-1</v>
       </c>
@@ -1729,7 +1734,7 @@
         <v>2.726</v>
       </c>
     </row>
-    <row r="58" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:7">
       <c r="B58">
         <v>0</v>
       </c>
@@ -1749,39 +1754,39 @@
         <v>2.59</v>
       </c>
     </row>
-    <row r="59" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B59" s="5" t="s">
+    <row r="59" spans="2:7">
+      <c r="B59" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C59" s="7">
+      <c r="C59" s="6">
         <f>SLOPE(D46:D58,B46:B58)</f>
         <v>-0.13815789473684209</v>
       </c>
-      <c r="D59" s="7">
+      <c r="D59" s="6">
         <f>SLOPE(D46:D58,C46:C58)</f>
         <v>0.13868029342668386</v>
       </c>
-      <c r="E59" s="5" t="s">
+      <c r="E59" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="F59" s="7">
+      <c r="F59" s="6">
         <f>SLOPE(G46:G58,E46:E58)</f>
         <v>-0.1355526315789474</v>
       </c>
-      <c r="G59" s="7">
+      <c r="G59" s="6">
         <f>SLOPE(G46:G58,F46:F58)</f>
         <v>0.13561418029572037</v>
       </c>
     </row>
-    <row r="60" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B60" s="5"/>
+    <row r="60" spans="2:7">
+      <c r="B60" s="4"/>
       <c r="C60" t="s">
         <v>2</v>
       </c>
       <c r="D60" t="s">
         <v>3</v>
       </c>
-      <c r="E60" s="5"/>
+      <c r="E60" s="4"/>
       <c r="F60" t="s">
         <v>2</v>
       </c>
@@ -1789,8 +1794,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="61" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B61" s="5" t="s">
+    <row r="61" spans="2:7">
+      <c r="B61" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C61">
@@ -1801,7 +1806,7 @@
         <f>RSQ(D46:D58,C46:C58)</f>
         <v>0.99960371242500834</v>
       </c>
-      <c r="E61" s="5" t="s">
+      <c r="E61" s="4" t="s">
         <v>4</v>
       </c>
       <c r="F61">
@@ -1813,72 +1818,72 @@
         <v>0.99998080711141257</v>
       </c>
     </row>
-    <row r="62" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B62" s="5" t="s">
+    <row r="62" spans="2:7">
+      <c r="B62" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C62">
-        <v>-0.12548418972332015</v>
+        <v>-0.13711495535714288</v>
       </c>
       <c r="D62">
-        <v>0.12608102115425956</v>
-      </c>
-      <c r="E62" s="5" t="s">
+        <v>0.13783328328485747</v>
+      </c>
+      <c r="E62" s="4" t="s">
         <v>5</v>
       </c>
       <c r="F62">
-        <v>-0.40648800000000013</v>
+        <v>-0.13732254464285715</v>
       </c>
       <c r="G62">
-        <v>0.40890683932975469</v>
-      </c>
-    </row>
-    <row r="63" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B63" s="5" t="s">
+        <v>0.13748322978580291</v>
+      </c>
+    </row>
+    <row r="63" spans="2:7">
+      <c r="B63" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C63">
         <f>C59-C62</f>
-        <v>-1.2673705013521941E-2</v>
+        <v>-1.0429393796992092E-3</v>
       </c>
       <c r="D63">
         <f>D59-D62</f>
-        <v>1.25992722724243E-2</v>
-      </c>
-      <c r="E63" s="5" t="s">
+        <v>8.4701014182639311E-4</v>
+      </c>
+      <c r="E63" s="4" t="s">
         <v>9</v>
       </c>
       <c r="F63">
         <f>F59-F62</f>
-        <v>0.2709353684210527</v>
+        <v>1.7699130639097505E-3</v>
       </c>
       <c r="G63">
         <f>G59-G62</f>
-        <v>-0.27329265903403432</v>
-      </c>
-    </row>
-    <row r="64" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B64" s="5" t="s">
+        <v>-1.8690494900825416E-3</v>
+      </c>
+    </row>
+    <row r="64" spans="2:7">
+      <c r="B64" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C64" s="2">
+      <c r="C64" s="1">
         <f>(C62-C59)/((C59+C62)/2)</f>
-        <v>-9.6143262100759241E-2</v>
-      </c>
-      <c r="D64" s="2">
+        <v>-7.5774954147720995E-3</v>
+      </c>
+      <c r="D64" s="1">
         <f>(D62-D59)/((D59+D62)/2)</f>
-        <v>-9.5174571046121786E-2</v>
-      </c>
-      <c r="E64" s="5" t="s">
+        <v>-6.1263548206169508E-3</v>
+      </c>
+      <c r="E64" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F64" s="2">
+      <c r="F64" s="1">
         <f>(F62-F59)/((F59+F62)/2)</f>
-        <v>0.99968656457294125</v>
-      </c>
-      <c r="G64" s="2">
+        <v>1.2972327409299333E-2</v>
+      </c>
+      <c r="G64" s="1">
         <f>(G62-G59)/((G59+G62)/2)</f>
-        <v>1.0037910353653812</v>
+        <v>1.368778627028799E-2</v>
       </c>
     </row>
   </sheetData>
@@ -1891,7 +1896,12 @@
     <mergeCell ref="E44:G44"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1903,25 +1913,25 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="17.7109375" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" customWidth="1"/>
-    <col min="4" max="4" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.6640625" customWidth="1"/>
+    <col min="3" max="3" width="10.5" customWidth="1"/>
+    <col min="4" max="4" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:5">
+      <c r="B1" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1" t="s">
+      <c r="C1" s="8"/>
+      <c r="D1" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="1"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E1" s="8"/>
+    </row>
+    <row r="2" spans="1:5">
       <c r="B2" t="s">
         <v>19</v>
       </c>
@@ -1935,7 +1945,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -1952,11 +1962,11 @@
         <v>-7.7640000000000002</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="2">
         <v>-72.400000000000006</v>
       </c>
       <c r="C4">
@@ -1969,7 +1979,7 @@
         <v>-7.4539999999999997</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -1986,7 +1996,7 @@
         <v>-7.6589999999999998</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -2003,7 +2013,7 @@
         <v>-7.6289999999999996</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -2016,11 +2026,11 @@
       <c r="D7">
         <v>70.91</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="3">
         <v>-7.28</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -2044,6 +2054,11 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -2053,8 +2068,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>